<commit_message>
Working on 8 and 9
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/483805976292d47c/Documents/NSS/excel/da16-lookups-exercise-janvimehendale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="944" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1A3123F-65DB-4DDB-80E9-8B168726564D}"/>
+  <xr:revisionPtr revIDLastSave="952" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25F8A7E-E084-4CA2-BD7E-70C00D4A41D8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1538,6 +1538,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="75000"/>
@@ -1570,6 +1573,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -1636,13 +1642,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -1766,13 +1773,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -1895,6 +1903,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="75000"/>
@@ -1966,6 +1977,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="75000"/>
@@ -2013,6 +2027,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -2043,28 +2060,36 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
         </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
+        <a:gs pos="74000">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="45000"/>
+            <a:lumOff val="55000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="83000">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="45000"/>
+            <a:lumOff val="55000"/>
+          </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="30000"/>
+            <a:lumOff val="70000"/>
           </a:schemeClr>
         </a:gs>
       </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
+      <a:lin ang="5400000" scaled="1"/>
       <a:tileRect/>
     </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2075,7 +2100,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3115,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6565,11 +6594,11 @@
         <f t="shared" si="12"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C79" s="13">
+      <c r="C79" s="23">
         <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D79" s="43">
+      <c r="D79" s="47">
         <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>

</xml_diff>